<commit_message>
Progress from today- resuming summary of studies
</commit_message>
<xml_diff>
--- a/meta-analysis/study summary.xlsx
+++ b/meta-analysis/study summary.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="6320" windowWidth="25280" windowHeight="15300" tabRatio="500"/>
+    <workbookView xWindow="40" yWindow="6120" windowWidth="25280" windowHeight="9500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="study_overall" sheetId="2" r:id="rId1"/>
+    <sheet name="interactions" sheetId="1" r:id="rId2"/>
+    <sheet name="notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="164">
   <si>
     <t>define match</t>
   </si>
@@ -245,13 +247,289 @@
   </si>
   <si>
     <t>zooplankton</t>
+  </si>
+  <si>
+    <t>aquatic (marine)</t>
+  </si>
+  <si>
+    <t>fitness (first sentence of introduction)</t>
+  </si>
+  <si>
+    <t>Great tit (Oxford)</t>
+  </si>
+  <si>
+    <t>Winter moth</t>
+  </si>
+  <si>
+    <t>population biomass (50% caterpillar fall date)</t>
+  </si>
+  <si>
+    <t>not measured</t>
+  </si>
+  <si>
+    <t>life-history</t>
+  </si>
+  <si>
+    <t>mammal</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>individual (calving date)</t>
+  </si>
+  <si>
+    <t>community (proportion of plant species emergent on the dae of 50 % caribou births)</t>
+  </si>
+  <si>
+    <t>community (annual date of 50% plant species emergent for each year)</t>
+  </si>
+  <si>
+    <t>individual (calf production)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author comments on strength or specialization of interaction </t>
+  </si>
+  <si>
+    <t>year range</t>
+  </si>
+  <si>
+    <t>1993, 2002-2011</t>
+  </si>
+  <si>
+    <t>10-14 years; 1999-2008</t>
+  </si>
+  <si>
+    <t>yes- Quantified what proportion of flower visits were from each species</t>
+  </si>
+  <si>
+    <t>phenofreq</t>
+  </si>
+  <si>
+    <t>not specified</t>
+  </si>
+  <si>
+    <t>first flowering</t>
+  </si>
+  <si>
+    <t>interaction type</t>
+  </si>
+  <si>
+    <t>pollination</t>
+  </si>
+  <si>
+    <t>marine</t>
+  </si>
+  <si>
+    <t>herbivory</t>
+  </si>
+  <si>
+    <t>27 years; 1985-2011</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Is Cushing only ever mentioned by name in aquatic studies?</t>
+  </si>
+  <si>
+    <t>Is food web theory only a mechanism relevant to aquatic studies?</t>
+  </si>
+  <si>
+    <t>individual (birth date)</t>
+  </si>
+  <si>
+    <t>community (mean date of flowering of vineyards)</t>
+  </si>
+  <si>
+    <t>individual (survival, fitness)</t>
+  </si>
+  <si>
+    <t>study_type</t>
+  </si>
+  <si>
+    <t>observational</t>
+  </si>
+  <si>
+    <t>HMK027</t>
+  </si>
+  <si>
+    <t>experimental</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>EXCLUDE ?</t>
+  </si>
+  <si>
+    <t>HMK028</t>
+  </si>
+  <si>
+    <t>population structure, community structure</t>
+  </si>
+  <si>
+    <t>insect (dragonfly)</t>
+  </si>
+  <si>
+    <t>predation</t>
+  </si>
+  <si>
+    <t>aquatic (freshwater)</t>
+  </si>
+  <si>
+    <t>predation (intraguild)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>22 years; 1986-2011</t>
+  </si>
+  <si>
+    <t>Cushing OR mismatch</t>
+  </si>
+  <si>
+    <t>includes list of species composition of community</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>community (onset of spring (*estimated from temperature))</t>
+  </si>
+  <si>
+    <t>population (size)</t>
+  </si>
+  <si>
+    <t>individual (fledged chicks)</t>
+  </si>
+  <si>
+    <t>individual (birth date but *estimated from when young was seen)</t>
+  </si>
+  <si>
+    <t>17 years; 1996-2013</t>
+  </si>
+  <si>
+    <t>no but cites Miller-Rushing et al. 2010</t>
+  </si>
+  <si>
+    <t>life-history (and envt?)</t>
+  </si>
+  <si>
+    <t>none but measured whole community so can't be specialist and includes entire diet!</t>
+  </si>
+  <si>
+    <t>arthropod</t>
+  </si>
+  <si>
+    <t>mentions that measure of arthropod is closely related to growth of arctic shorebird chicks (doesn't specify species); also--We included all specimens in the orders of these group X, Y, Z, which have been shown to be part of the diet of Sanderlings in Zackenberg</t>
+  </si>
+  <si>
+    <t>individual (hatch date but *modeled)</t>
+  </si>
+  <si>
+    <t>community (date of median abundance)</t>
+  </si>
+  <si>
+    <t>individual (body mass)</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>invertebrate (bivalve)</t>
+  </si>
+  <si>
+    <t>29 years; 1973-2001</t>
+  </si>
+  <si>
+    <t>mechanism (implicit)</t>
+  </si>
+  <si>
+    <t>we analyze the combined effects of the temperature-related environmental variables (viz.
+time and magnitude of food availability, time and magnitude
+of predatory shrimps, advection of larvae toward the open
+sea, and interference by cockle stock) on the instantaneous
+mortality rate</t>
+  </si>
+  <si>
+    <t>food web if multiple factors?</t>
+  </si>
+  <si>
+    <t>invertebrate (shrimp)</t>
+  </si>
+  <si>
+    <t>food web? Life history?</t>
+  </si>
+  <si>
+    <t>How to determine mechanism?</t>
+  </si>
+  <si>
+    <t>phytoplankton was 1-2/month to 1-2/week in spring</t>
+  </si>
+  <si>
+    <t>plant (phytoplankton)</t>
+  </si>
+  <si>
+    <t>community (peak of spring bloom (derived from normal density function))</t>
+  </si>
+  <si>
+    <t>abiotic or population (timing of spawning (modeled based on min threshold temp))</t>
+  </si>
+  <si>
+    <t>population (peak predation pressure (derived from normal density function))</t>
+  </si>
+  <si>
+    <t>individual (reproductive output (eggs m2))</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>9  years; 2005-2013</t>
+  </si>
+  <si>
+    <t>int_id</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bird (brood parasite)</t>
+  </si>
+  <si>
+    <t>parasitism (brood)</t>
+  </si>
+  <si>
+    <t>individual (lay date)</t>
+  </si>
+  <si>
+    <t>population (number ofparasitized nests/total number of nests)</t>
+  </si>
+  <si>
+    <t>bird (host is magpie)</t>
+  </si>
+  <si>
+    <t>interaction strength- any evidence that relationship with resource affects consumer's fitness? (independent of phenology)</t>
+  </si>
+  <si>
+    <t>specialized interaction between some obligate avian brood parasites (hereafter cuckoos) and some of their favourite hosts; Cuckoo parasitism reduces magpie reproductive
+success by 80.0% through early hatching and eff ective
+competition for parental food delivery of cuckoo nestlings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -288,13 +566,67 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -306,7 +638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -336,8 +668,120 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -354,8 +798,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="141">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +844,62 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -384,6 +914,62 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -713,430 +1299,511 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="4"/>
+    <col min="2" max="2" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>4</v>
+        <v>140</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>93</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="4">
-        <v>1</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="4">
-        <v>1</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L6" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="4">
-        <v>1</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="B9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="1" t="s">
+      <c r="H10" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="B12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="B14" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="B15" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="B24" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="B25" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="B26" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="B28" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="B29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="30">
       <c r="A30" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="B30" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="B31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="G32" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1147,4 +1814,733 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" s="6">
+        <v>1</v>
+      </c>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="F35" s="13"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="D39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Progress from Oct 25- Adding review component to ms and organization of ms
</commit_message>
<xml_diff>
--- a/meta-analysis/study summary.xlsx
+++ b/meta-analysis/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="6120" windowWidth="25280" windowHeight="9500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3980" yWindow="0" windowWidth="22520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="study_overall" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="205">
   <si>
     <t>define match</t>
   </si>
@@ -523,6 +523,137 @@
     <t>specialized interaction between some obligate avian brood parasites (hereafter cuckoos) and some of their favourite hosts; Cuckoo parasitism reduces magpie reproductive
 success by 80.0% through early hatching and eff ective
 competition for parental food delivery of cuckoo nestlings</t>
+  </si>
+  <si>
+    <t>indirectly- Great tits rely on caterpillars to feed their chicks
+and strive to match their breeding time with the
+pronounced seasonal peak in caterpillar biomass,
+which enhances offspring surviva</t>
+  </si>
+  <si>
+    <t>individual (lay date of first clutch)</t>
+  </si>
+  <si>
+    <t>community (peak abundance estimated)</t>
+  </si>
+  <si>
+    <t>38 years; 1973-2011</t>
+  </si>
+  <si>
+    <t>individual (mean adult survival per year, mean number of fledglings per female per season), population (number)</t>
+  </si>
+  <si>
+    <t>9 years; 1997-2006</t>
+  </si>
+  <si>
+    <t>fish (salmon)</t>
+  </si>
+  <si>
+    <t>first arrival of any salmon</t>
+  </si>
+  <si>
+    <t>population (first appearance based on daily census counts)</t>
+  </si>
+  <si>
+    <t>population (peak abundance)</t>
+  </si>
+  <si>
+    <t>an opportunistic predator, feed heavily on salmon eggs. Where salmon remain at historical levels of abundance, Dolly Varden can acquire the majority of their annual energy intake by gorging on salmon eggs</t>
+  </si>
+  <si>
+    <t>yes- abundance</t>
+  </si>
+  <si>
+    <t>food web? Analyze multiple factors</t>
+  </si>
+  <si>
+    <t>Understanding the mechanisms responsible for recruitment variation</t>
+  </si>
+  <si>
+    <t>arthropod (crustacean, copepod)= zooplankton</t>
+  </si>
+  <si>
+    <t>yes- Copepods are the major prey of sandeel larvae, with A. marinus
+exhibiting an increasing selectivity towards Calanus
+finmarchicus by the late larval stage in the northern
+North Sea. However, in much of
+the North Sea, C. helgolandicus is the most dominant
+large calanoid copepod</t>
+  </si>
+  <si>
+    <t>individual BUT estimated based on number of increments on otolith and subtracted from capture date</t>
+  </si>
+  <si>
+    <t>7 years; 1999-2003, 2009, 2013</t>
+  </si>
+  <si>
+    <t>individual but not indpedent (date of maximum egg production estimated based on size distribution)</t>
+  </si>
+  <si>
+    <t>population (abundance)</t>
+  </si>
+  <si>
+    <t>HMK009</t>
+  </si>
+  <si>
+    <t>* NDVI used to predict peak nitrogen for some years, can we only use years where peak nitrogen measured??  peak nitrogen for plants BUT</t>
+  </si>
+  <si>
+    <t>HMK010</t>
+  </si>
+  <si>
+    <t>* NDVI used to predict date of peak; previous search (2014)- no species or genus level data for second species (for graminoids)- peak nitrogen used for plants; NO- NDVI used to predict date of peak productivity</t>
+  </si>
+  <si>
+    <t>HMK021</t>
+  </si>
+  <si>
+    <t>* not sure species directly interact, "potential" used in paper, also families used</t>
+  </si>
+  <si>
+    <t>HMK051</t>
+  </si>
+  <si>
+    <t>previous search(2014); no raw data given!</t>
+  </si>
+  <si>
+    <t>recheck</t>
+  </si>
+  <si>
+    <t>no raw fitness data; uses temp sum instead of doy for plant phenology; relies on GDD as proxy for plant phenology</t>
+  </si>
+  <si>
+    <t>HMK024</t>
+  </si>
+  <si>
+    <t>no raw data porvided; survival/recruitment is modelled!;laying date (pheno provided) is estimated!! years not provided</t>
+  </si>
+  <si>
+    <t>HMK056</t>
+  </si>
+  <si>
+    <t>can't get pheno data for 5 years from paper (even though it's been analyxed; predicted phenology (back-calculations)</t>
+  </si>
+  <si>
+    <t>meta-analysis; modelled mismatch</t>
+  </si>
+  <si>
+    <t>only proportion of nests predated and breeding season length for performance; used breeding season length as proxy for reproductive capacity</t>
+  </si>
+  <si>
+    <t>only 4 years with food quality; resource availability indexed by N concentration</t>
+  </si>
+  <si>
+    <t>only showing data from NDVI not GDD; GDD used for plant phenology</t>
+  </si>
+  <si>
+    <t>no phenology data for second spp; phenology was estimated by thermal requirements</t>
+  </si>
+  <si>
+    <t>no fitness data; modelled phenology data using climate variables</t>
+  </si>
+  <si>
+    <t>no fitness data; used seaice breakup date as proxy for polar bear timing</t>
   </si>
 </sst>
 </file>
@@ -609,7 +740,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,6 +759,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -638,7 +781,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="141">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -780,8 +923,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -828,8 +1019,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="141">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -900,6 +1101,30 @@
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -970,6 +1195,30 @@
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1299,11 +1548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1311,7 +1560,8 @@
     <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="22.1640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
@@ -1627,6 +1877,18 @@
       <c r="B24" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C24" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
@@ -1635,13 +1897,46 @@
       <c r="B25" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="C25" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>108</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1803,6 +2098,160 @@
       </c>
       <c r="G34" s="4" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1818,188 +2267,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="2" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1">
+    <row r="1" spans="1:14" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="J2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="4">
         <v>1</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="K4" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="K4" s="4">
+      <c r="M4" s="4">
         <v>1</v>
       </c>
-      <c r="L4" s="4">
+      <c r="N4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>42</v>
@@ -2008,486 +2470,704 @@
         <v>42</v>
       </c>
       <c r="K5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="4">
         <v>1</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="J7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="4">
         <v>1</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="K10" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="K11" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14">
       <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="9"/>
+      <c r="J12" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="K13" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="B19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="B20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="B23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="B26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="1"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="I28" s="4" t="s">
+      <c r="K28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="1"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="G30" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="J30" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="K30" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="L30" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="C31" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="F31" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G31" s="16" t="s">
+      <c r="I31" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="J31" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="L31" s="4" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:12">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="K32" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="L32" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="H33" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="K33" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6" t="s">
+      <c r="H34" s="6"/>
+      <c r="I34" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="J34" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="K34" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="L34" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K34" s="6">
+      <c r="M34" s="6">
         <v>1</v>
       </c>
-      <c r="L34" s="6"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="F35" s="13"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="B35" s="1"/>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="1"/>
+      <c r="F39" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>115</v>
       </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>